<commit_message>
Small fix for saving data in trio test
Removed [] in saving data in rows plus new results for trio
</commit_message>
<xml_diff>
--- a/Results/Test_Powietrze_04_Drogi_04_Samochody_ciezar_04_kendall.xlsx
+++ b/Results/Test_Powietrze_04_Drogi_04_Samochody_ciezar_04_kendall.xlsx
@@ -473,28 +473,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>['POLSKA']</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>[-0.43859649122807015]</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>[0.9532163742690059]</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>[0.008263500509190905]</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>[1.1681522685453174e-13]</t>
-        </is>
+          <t>PODLASKIE</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.4385964912280702</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.8947368421052631</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.008263500509190905</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6.639132996608248e-11</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -506,31 +498,23 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>['POMORSKIE']</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>[0.3099415204678362]</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>[0.5672514619883041]</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>[0.06835950866699914]</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>[0.00042903433978188217]</t>
-        </is>
+          <t>MAZOWIECKIE</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.6608187134502924</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9064327485380117</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2.384192925441844e-05</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.279968523745518e-11</v>
       </c>
       <c r="F3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -539,28 +523,20 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>['LUBELSKIE']</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>[-0.14619883040935672]</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>[0.9181286549707602]</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>[0.40626461663128227]</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>[7.207968073133665e-12]</t>
-        </is>
+          <t>LUBUSKIE</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1695906432748538</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.847953216374269</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.3320065987053188</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.532332654292704e-09</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -572,94 +548,70 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>['LUBUSKIE']</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>[0.1695906432748538]</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>[0.847953216374269]</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>[0.33200659870531884]</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>[2.532332654292704e-09]</t>
-        </is>
+          <t>WARMIŃSKO-MAZURSKIE</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5906432748538012</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1812865497076024</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0002230758404187383</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.2983021854281703</v>
       </c>
       <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="b">
         <v>0</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>['ŚLĄSKIE']</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>[-0.6257309941520467]</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>[-0.06432748538011696]</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>[7.706900787983835e-05]</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>[0.7300327269910041]</t>
-        </is>
+          <t>KUJAWSKO-POMORSKIE</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.543859649122807</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.871345029239766</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0007930719198513941</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4.583225285081198e-10</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>['PODLASKIE']</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>[0.43859649122807015]</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>[0.894736842105263]</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>[0.008263500509190905]</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>[6.639132996608248e-11]</t>
-        </is>
+          <t>POLSKA</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-0.4385964912280702</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.9532163742690059</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.008263500509190905</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.168152268545317e-13</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -671,31 +623,23 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>['MAZOWIECKIE']</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>[0.6608187134502924]</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>[0.9064327485380117]</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>[2.3841929254418437e-05]</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>[2.2799685237455178e-11]</t>
-        </is>
+          <t>OPOLSKIE</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-0.4152046783625731</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.5339737003888005</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.01282401882734904</v>
       </c>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -704,61 +648,45 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>['ŚWIĘTOKRZYSKIE']</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>[0.5555555555555555]</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>[0.6491228070175439]</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>[0.0005861005055629151]</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>[3.572251772054519e-05]</t>
-        </is>
+          <t>ŚLĄSKIE</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.6257309941520467</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.06432748538011696</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7.706900787983835e-05</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.7300327269910041</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
       <c r="G9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>['WIELKOPOLSKIE']</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>[-0.8245614035087718]</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>[0.8596491228070176]</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>[1.1706731493614734e-08]</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>[1.1042535667161752e-09]</t>
-        </is>
+          <t>ZACHODNIOPOMORSKIE</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-0.5321637426900584</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.6023391812865496</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.001063322190259039</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0001583185669873452</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -770,28 +698,20 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>['DOLNOŚLĄSKIE']</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>[-0.6608187134502924]</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>[0.7894736842105262]</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>[2.3841929254418437e-05]</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>[8.90628326466768e-08]</t>
-        </is>
+          <t>MAŁOPOLSKIE</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-0.6608187134502924</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.7426900584795321</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2.384192925441844e-05</v>
+      </c>
+      <c r="E11" t="n">
+        <v>9.024576201675731e-07</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -803,31 +723,23 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>['OPOLSKIE']</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>[0.1111111111111111]</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>[-0.4152046783625731]</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>[0.5339737003888005]</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>[0.01282401882734904]</t>
-        </is>
+          <t>PODKARPACKIE</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-0.7309941520467835</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.9064327485380117</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.520915300379556e-06</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2.279968523745518e-11</v>
       </c>
       <c r="F12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -836,31 +748,23 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>['ŁÓDZKIE']</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>[0.3567251461988304]</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>[0.6257309941520467]</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>[0.034430960241941616]</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>[7.706900787983835e-05]</t>
-        </is>
+          <t>LUBELSKIE</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-0.1461988304093567</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.9181286549707602</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.4062646166312823</v>
+      </c>
+      <c r="E13" t="n">
+        <v>7.207968073133665e-12</v>
       </c>
       <c r="F13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -869,61 +773,45 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>['WARMIŃSKO-MAZURSKIE']</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>[0.5906432748538012]</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>[0.18128654970760236]</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>[0.00022307584041873825]</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>[0.2983021854281703]</t>
-        </is>
+          <t>POMORSKIE</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.3099415204678362</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.5672514619883041</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.06835950866699914</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.0004290343397818822</v>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>['ZACHODNIOPOMORSKIE']</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>[-0.5321637426900584]</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>[0.6023391812865496]</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>[0.0010633221902590392]</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>[0.0001583185669873452]</t>
-        </is>
+          <t>ŁÓDZKIE</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.3567251461988304</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.6257309941520467</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.03443096024194162</v>
+      </c>
+      <c r="E15" t="n">
+        <v>7.706900787983835e-05</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
@@ -935,28 +823,20 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>['PODKARPACKIE']</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>[-0.7309941520467835]</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>[0.9064327485380117]</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>[1.5209153003795562e-06]</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>[2.2799685237455178e-11]</t>
-        </is>
+          <t>WIELKOPOLSKIE</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-0.8245614035087718</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.8596491228070176</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.170673149361473e-08</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.104253566716175e-09</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
@@ -968,28 +848,20 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>['MAŁOPOLSKIE']</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>[-0.6608187134502924]</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>[0.7426900584795321]</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>[2.3841929254418437e-05]</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>[9.024576201675731e-07]</t>
-        </is>
+          <t>ŚWIĘTOKRZYSKIE</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.5555555555555555</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.6491228070175439</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0005861005055629151</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.572251772054519e-05</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
@@ -1001,28 +873,20 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>['KUJAWSKO-POMORSKIE']</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>[0.543859649122807]</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>[0.871345029239766]</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>[0.0007930719198513941]</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>[4.583225285081198e-10]</t>
-        </is>
+          <t>DOLNOŚLĄSKIE</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-0.6608187134502924</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.7894736842105262</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.384192925441844e-05</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8.90628326466768e-08</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>

</xml_diff>